<commit_message>
Removed unnecessary comments and debugs
</commit_message>
<xml_diff>
--- a/groups2.xlsx
+++ b/groups2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktana\PycharmProjects\python_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{698EE48B-3C2A-4688-8FFF-D25477F98EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3456ED97-ED13-4E8C-92E5-6AB65742EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2610" windowWidth="28800" windowHeight="15435" xr2:uid="{F4789E0B-65C3-4EA3-85EF-68C4EA799D5B}"/>
+    <workbookView xWindow="4950" yWindow="2610" windowWidth="28800" windowHeight="15435" xr2:uid="{8AD6ADA3-CD0E-4D24-A775-4B900CBB7129}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -44,40 +44,49 @@
     <t>Footer</t>
   </si>
   <si>
-    <t>N80240</t>
-  </si>
-  <si>
-    <t>H11730</t>
-  </si>
-  <si>
-    <t>F44661</t>
-  </si>
-  <si>
-    <t>N86558</t>
-  </si>
-  <si>
-    <t>H58004</t>
-  </si>
-  <si>
-    <t>F68069</t>
-  </si>
-  <si>
-    <t>N63173</t>
-  </si>
-  <si>
-    <t>H86453</t>
-  </si>
-  <si>
-    <t>F46494</t>
-  </si>
-  <si>
-    <t>N98227</t>
-  </si>
-  <si>
-    <t>H95999</t>
-  </si>
-  <si>
-    <t>F11563</t>
+    <t>N79426</t>
+  </si>
+  <si>
+    <t>H04145</t>
+  </si>
+  <si>
+    <t>F35309</t>
+  </si>
+  <si>
+    <t>N15841</t>
+  </si>
+  <si>
+    <t>H96890</t>
+  </si>
+  <si>
+    <t>F53433</t>
+  </si>
+  <si>
+    <t>N75760</t>
+  </si>
+  <si>
+    <t>H26944</t>
+  </si>
+  <si>
+    <t>F09486</t>
+  </si>
+  <si>
+    <t>N69119</t>
+  </si>
+  <si>
+    <t>H54520</t>
+  </si>
+  <si>
+    <t>F75957</t>
+  </si>
+  <si>
+    <t>N08908</t>
+  </si>
+  <si>
+    <t>H56185</t>
+  </si>
+  <si>
+    <t>F65173</t>
   </si>
 </sst>
 </file>
@@ -429,8 +438,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3DBE70-FAFD-4554-82A6-4AB14CCABD30}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EDE853-D95F-40EA-A70B-1962B5333041}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,6 +500,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>